<commit_message>
Capacita - aprovacao de cursos
</commit_message>
<xml_diff>
--- a/Necessidades.xlsx
+++ b/Necessidades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Descricao</t>
   </si>
@@ -46,19 +46,25 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>Teste1</t>
-  </si>
-  <si>
-    <t>Begin</t>
-  </si>
-  <si>
-    <t>iniciativa1</t>
-  </si>
-  <si>
-    <t>baixo</t>
-  </si>
-  <si>
-    <t>Analise</t>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>Senado</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Teoria da Comunicação</t>
+  </si>
+  <si>
+    <t>facil</t>
+  </si>
+  <si>
+    <t>Matutino</t>
+  </si>
+  <si>
+    <t>Dezembro</t>
   </si>
   <si>
     <t>medio</t>
@@ -67,37 +73,40 @@
     <t>Vespertino</t>
   </si>
   <si>
-    <t>Agosto</t>
-  </si>
-  <si>
-    <t>Teste2</t>
-  </si>
-  <si>
-    <t>Lorem</t>
-  </si>
-  <si>
-    <t>médio</t>
-  </si>
-  <si>
-    <t>Administração de Recursos Humanos</t>
-  </si>
-  <si>
-    <t>Matutino</t>
-  </si>
-  <si>
-    <t>Teste3</t>
-  </si>
-  <si>
-    <t>alta</t>
-  </si>
-  <si>
-    <t>Geometria e Topologia</t>
-  </si>
-  <si>
-    <t>facil</t>
-  </si>
-  <si>
-    <t>Julho</t>
+    <t>Junho</t>
+  </si>
+  <si>
+    <t>bligs blaps</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Sociologia Jurídica</t>
+  </si>
+  <si>
+    <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>joop joops</t>
+  </si>
+  <si>
+    <t>Teoria do Estado</t>
+  </si>
+  <si>
+    <t>Março</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topicos em negocios internacionais </t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Negócios Internacionais</t>
+  </si>
+  <si>
+    <t>Novembro</t>
   </si>
 </sst>
 </file>
@@ -443,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,99 +495,189 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2">
-        <v>30</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="20" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E5" s="2">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2">
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Capacita - relatorio agregando cursos
</commit_message>
<xml_diff>
--- a/Necessidades.xlsx
+++ b/Necessidades.xlsx
@@ -43,34 +43,55 @@
     <t>Custo</t>
   </si>
   <si>
+    <t>kjhlkjh</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Biblioteconomia</t>
+  </si>
+  <si>
+    <t>Avançado</t>
+  </si>
+  <si>
+    <t>Seminário</t>
+  </si>
+  <si>
+    <t>brunocordeiro180</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Teoria da Comunicação</t>
+  </si>
+  <si>
+    <t>Intermediário</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
     <t>Tópicos em Serviço Social de Educação</t>
   </si>
   <si>
-    <t>Média</t>
-  </si>
-  <si>
     <t>Serviço Social da Educação</t>
   </si>
   <si>
     <t>Básico</t>
   </si>
   <si>
-    <t>Workshop</t>
-  </si>
-  <si>
-    <t>brunocordeiro180</t>
-  </si>
-  <si>
     <t>owo</t>
   </si>
   <si>
     <t>Componentes da Dinâmica Demográfica</t>
   </si>
   <si>
-    <t>Intermediário</t>
-  </si>
-  <si>
-    <t>Palestra</t>
+    <t>Curso</t>
   </si>
   <si>
     <t>dfasadsf</t>
@@ -79,46 +100,25 @@
     <t>Contabilidade Nacional</t>
   </si>
   <si>
-    <t>Avançado</t>
-  </si>
-  <si>
-    <t>kjhlkjh</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>Biblioteconomia</t>
-  </si>
-  <si>
-    <t>Seminário</t>
+    <t>nupcidade</t>
+  </si>
+  <si>
+    <t>Nupcialidade e Família</t>
+  </si>
+  <si>
+    <t>kgkkjhkjh</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Conflitos e Coalizões Políticas</t>
   </si>
   <si>
     <t>asdafd</t>
   </si>
   <si>
     <t>Inflação</t>
-  </si>
-  <si>
-    <t>kgkkjhkjh</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Conflitos e Coalizões Políticas</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Teoria da Comunicação</t>
-  </si>
-  <si>
-    <t>nupcidade</t>
-  </si>
-  <si>
-    <t>Nupcialidade e Família</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -520,7 +520,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
@@ -529,7 +529,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="2">
-        <v>250</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20" customHeight="1">
@@ -537,77 +537,77 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
         <v>17</v>
       </c>
-      <c r="F3" s="2">
-        <v>3</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="2">
-        <v>100</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>88</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="2">
-        <v>456</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -624,10 +624,10 @@
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>27</v>
@@ -636,16 +636,16 @@
         <v>12</v>
       </c>
       <c r="F6" s="2">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="2">
-        <v>100</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1">
@@ -653,36 +653,36 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="2">
-        <v>852</v>
+        <v>567.23</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -691,10 +691,10 @@
         <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>25</v>
@@ -703,7 +703,7 @@
         <v>14</v>
       </c>
       <c r="I8" s="2">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20" customHeight="1">
@@ -711,19 +711,19 @@
         <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -732,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="2">
-        <v>567.23</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insercao de usuario arrumada
</commit_message>
<xml_diff>
--- a/Necessidades.xlsx
+++ b/Necessidades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Sugestão de Curso</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Custo</t>
   </si>
   <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
@@ -143,6 +146,12 @@
   </si>
   <si>
     <t>amoedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">midia training </t>
+  </si>
+  <si>
+    <t>Marketing</t>
   </si>
   <si>
     <t>tec da arquitetura</t>
@@ -494,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,7 +513,7 @@
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" customHeight="1">
+    <row r="1" spans="1:10" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,411 +541,488 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2">
         <v>956</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1">
+      <c r="J2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1">
+      <c r="J3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2">
         <v>456</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1">
+      <c r="J4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1">
+      <c r="J5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2">
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1">
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2">
         <v>852</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1">
+      <c r="J7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2">
         <v>567.23</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1">
+      <c r="J8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2">
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1">
+      <c r="J9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2">
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="2">
         <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1">
+      <c r="J10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" s="2">
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I11" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1">
+      <c r="J11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1">
+      <c r="J12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2">
         <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2">
         <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1">
+      <c r="J13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2">
+        <v>88</v>
+      </c>
+      <c r="J14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="20" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="2">
-        <v>12</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I15" s="2">
         <v>100</v>
+      </c>
+      <c r="J15" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="20" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="2">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="2">
+        <v>100</v>
+      </c>
+      <c r="J16" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>